<commit_message>
sub avg for missing half-lifes in degrads
</commit_message>
<xml_diff>
--- a/tests/fixtures/min_kb.xlsx
+++ b/tests/fixtures/min_kb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="552" windowWidth="28476" windowHeight="12108" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="135" yWindow="555" windowWidth="28470" windowHeight="12105" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -1946,7 +1946,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2022,16 +2022,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
@@ -2086,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2111,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2136,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2161,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2186,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2211,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2236,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2261,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2311,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2336,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2360,9 +2363,7 @@
       <c r="F13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
@@ -2386,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2411,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2436,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2461,7 +2462,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -2486,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2511,7 +2512,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -2536,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -2561,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2586,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2611,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -2636,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2661,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2686,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2711,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -2736,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2761,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2786,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2811,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2836,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2861,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2883,9 +2884,9 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -2958,9 +2959,9 @@
       <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -4222,9 +4223,9 @@
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -4267,9 +4268,9 @@
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -4315,9 +4316,9 @@
       <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -4416,9 +4417,9 @@
       <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -4661,14 +4662,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4695,7 +4696,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4740,9 +4741,9 @@
       <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -4805,9 +4806,9 @@
       <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -5326,7 +5327,7 @@
       <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5392,7 +5393,7 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5446,7 +5447,7 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -6199,10 +6200,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -6480,9 +6484,7 @@
       <c r="F11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="2">
-        <v>115.5909672809378</v>
-      </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
@@ -6656,7 +6658,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>86.540087745138806</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -6928,7 +6930,7 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">

</xml_diff>